<commit_message>
Added support for Excel
</commit_message>
<xml_diff>
--- a/jira_time_logs_2025_05.xlsx
+++ b/jira_time_logs_2025_05.xlsx
@@ -7,7 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Time Logs" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Hours by Person" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Hours by Ticket" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1618,4 +1620,901 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Assignee</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Hours Logged</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Alfaz Jikani</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>32.75</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Bernardo Gallo Victorino dos Santos</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Eduardo Evangelista</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Fedor Biriukov</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Gabriel Guimaraes</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Ivo Parun Rua</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>João Nascimento</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Layne Silveira</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Lucas Dias</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Luciano Palmieri</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>33.67</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Oleg Akimov</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Renato Nunes</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Sergey Klochkov</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>david.burke</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Ticket Number</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Ticket Description</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Hours Logged</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>TR-9225</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>ADD search bar and enhanced formatting for linking a Data Set</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>TR-13098</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>API on Cellar for CodeGen application</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>TR-12304</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Add ability to support Oracle as a database type (several versions)</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>TR-12199</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>Add examples and details in Salesforce Rules documentation.</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>TR-12927</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>Add filters on Admin &gt; Combinator Activity Stats page</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>TR-12330</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>Allow refactor out selected lines of code into rules (also refactor out from other test cases/rules)</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>TR-13104</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>Android test cases stuck in queue for a long time</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>TR-9273</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>BLOCKER: Tests are taking a long time in the status queue/setting up while servers are available</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>TR-12385</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>BLOCKER: Unable to Upload File Using Enter and Drag Command</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>TR-8838</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>CRASH: Error of setting geolocation permissions on iOS app startup [iOS, x86_64]</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>TR-13069</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>CRASH: Major code leak inside error message</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>TR-13047</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>CRITICAL : 'Enter Data' Dropdown Remains Persistently Open During Automation, Causing Subsequent Test Step Failures</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>TR-12380</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>CRITICAL : Double-clicking the "Retest" button on the Test cases page triggers two concurrent executions of the same test case, resulting in the allocation of two servers</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>TR-12868</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>CRTICAL : Test suite run is not progressing immediately beyond the execution of the 'Before Suite' hook</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>TR-12624</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>Clicking on the screen in live mode should have option to generate ai-based commands</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>TR-12836</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>CodeGen</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>TR-8835</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>CodeGen      create loop to get new tasks</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>TR-13073</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>Combinator crash on JDBC init [Java 21]</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>TR-12692</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>Display the Value of Stored Value variables on Fail, not just the Key</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>TR-12413</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>Do not trust SAML email</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>TR-12827</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>FEATURE: Preserve Test Case Management Link When Copying Existing Test Cases Between Suites</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>TR-13066</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>Files are not downloaded and test cases are crashing</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>TR-13094</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>Filling out form crashes with "Form is no longer on the page"</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>TR-12452</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>Find &amp; Replace Enhancements - Display Suite Name &amp; Indicate Progress of Search</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>TR-8197</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>Full Spanish Support</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>TR-12409</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>INVESTIGATION : Pass Percentage Decrease After Re-running Failed Test Cases in EDCAST Baseline Run</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>TR-12588</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>Ignore hanging servers when calculating organization's server usage</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>TR-8842</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>Improve stability of test steps generation with AI</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>TR-8723</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>Introduce read-only role</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>TR-12518</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>Make default settings for plan NOT archived and Private</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>TR-13077</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>Oleg - Time Recording - Burnt</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>TR-13076</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>Oleg - Time Recording - Management</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>TR-12231</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>Orka trial</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>TR-12532</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>Pre-filter Accessibility standards in Settings to not to even catch others</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>TR-11872</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>Reference history of original test case/rule</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>TR-8791</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>Rollout iOS 18 support</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>TR-12558</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>Sales Blocker: Unable to zoom or pinch on map in mobile application - inKind</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>TR-13082</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>Some prod Macs offline for a while</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>TR-12324</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>The button icon (after "Work Item in Azure DevOps") is displayed outside the boundaries of the button</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>TR-13049</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>Time Recording : Meetings</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>TR-13050</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>Time Recording: Interviews</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>TR-13052</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Time Recording: Mentoring </t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>TR-13051</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>Time Recording: PR Reviews</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>11.75</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>TR-13074</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>Time Recording: Support assistance</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>TR-8845</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>UX Improvement: When a click is performed in LIVE mode from Debug, add the statement at the cursor, not the bottom of the page, to accelerate debugging.</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>TR-8760</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>Update host macOS, VM macOS and Parallels Desktop for Apple Silicon</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>